<commit_message>
Had to write a loop for the FIFO, derived measures may no longer be correct
</commit_message>
<xml_diff>
--- a/Case 1/Case 1 - dummy data.xlsx
+++ b/Case 1/Case 1 - dummy data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5509842B-0867-8B45-BAF8-BDB34A80D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B4678-CD1A-7F47-B064-CCD8D229DF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
   <si>
     <t>INFRASTRUCTURE</t>
   </si>
@@ -588,57 +588,13 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>TimetableComplete!$J$4:$J$25</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>IC</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>IC</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>IC</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>IC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1849,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y115"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1911,7 +1867,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T8" t="s">
         <v>6</v>
@@ -1947,7 +1903,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -2327,7 +2283,7 @@
         <v>32</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="U69" t="s">
         <v>33</v>
@@ -2338,7 +2294,7 @@
         <v>34</v>
       </c>
       <c r="B70">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
@@ -2674,10 +2630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2687,7 +2643,7 @@
     <col min="5" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -2709,433 +2665,205 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>42</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>52</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>48</v>
       </c>
-      <c r="E3" s="1">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3</v>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>58</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="1">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>54</v>
-      </c>
-      <c r="E4" s="1">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L6" s="1">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
+      <c r="O6" s="1">
+        <v>42</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5</v>
+      </c>
+      <c r="O7" s="1">
+        <v>48</v>
+      </c>
+      <c r="P7" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L8" s="1">
+        <v>13</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1">
+        <v>54</v>
+      </c>
+      <c r="P8" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="M10" t="s">
         <v>66</v>
       </c>
-      <c r="C6">
+      <c r="N10">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="O10">
         <v>40</v>
       </c>
-      <c r="E6">
+      <c r="P10">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="Q10">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L11">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="M11" t="s">
         <v>66</v>
       </c>
-      <c r="C7">
+      <c r="N11">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="Q11">
         <v>12</v>
       </c>
-      <c r="J7" s="1">
-        <v>12</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="1">
-        <v>5</v>
-      </c>
-      <c r="M7" s="1">
-        <v>50</v>
-      </c>
-      <c r="N7" s="1">
-        <v>6</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J8">
-        <v>12</v>
-      </c>
-      <c r="K8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
-      <c r="M8">
-        <v>58</v>
-      </c>
-      <c r="N8">
-        <v>6</v>
-      </c>
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J9" s="1">
-        <v>13</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" s="1">
-        <v>6</v>
-      </c>
-      <c r="M9" s="1">
-        <v>6</v>
-      </c>
-      <c r="N9" s="1">
-        <v>6</v>
-      </c>
-      <c r="O9" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J10" s="1">
-        <v>13</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" s="1">
-        <v>6</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1">
-        <v>6</v>
-      </c>
-      <c r="O10" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L11">
-        <v>5</v>
-      </c>
-      <c r="M11">
-        <v>42</v>
-      </c>
-      <c r="N11">
-        <v>5</v>
-      </c>
-      <c r="O11">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12">
-        <v>5</v>
-      </c>
-      <c r="M12">
-        <v>40</v>
-      </c>
-      <c r="N12">
-        <v>5</v>
-      </c>
-      <c r="O12">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="K13" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13">
-        <v>5</v>
-      </c>
-      <c r="M13">
-        <v>46</v>
-      </c>
-      <c r="N13">
-        <v>5</v>
-      </c>
-      <c r="O13">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J16" s="1">
-        <v>12</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="1">
-        <v>5</v>
-      </c>
-      <c r="M16" s="1">
-        <v>55</v>
-      </c>
-      <c r="N16" s="1">
-        <v>6</v>
-      </c>
-      <c r="O16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="J17">
-        <v>13</v>
-      </c>
-      <c r="K17" t="s">
-        <v>66</v>
-      </c>
-      <c r="L17">
-        <v>5</v>
-      </c>
-      <c r="M17">
-        <v>58</v>
-      </c>
-      <c r="N17">
-        <v>6</v>
-      </c>
-      <c r="O17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="J18" s="1">
-        <v>13</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18" s="1">
-        <v>5</v>
-      </c>
-      <c r="M18" s="1">
-        <v>59</v>
-      </c>
-      <c r="N18" s="1">
-        <v>6</v>
-      </c>
-      <c r="O18" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="J19" s="1">
-        <v>12</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" s="1">
-        <v>6</v>
-      </c>
-      <c r="M19" s="1">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1">
-        <v>6</v>
-      </c>
-      <c r="O19" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="I22">
-        <v>2</v>
-      </c>
-      <c r="J22" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22">
-        <v>5</v>
-      </c>
-      <c r="L22">
-        <v>40</v>
-      </c>
-      <c r="M22">
-        <v>5</v>
-      </c>
-      <c r="N22">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="I23">
-        <v>12</v>
-      </c>
-      <c r="J23" t="s">
-        <v>66</v>
-      </c>
-      <c r="K23">
-        <v>5</v>
-      </c>
-      <c r="L23">
-        <v>42</v>
-      </c>
-      <c r="M23">
-        <v>5</v>
-      </c>
-      <c r="N23">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="I24">
-        <v>3</v>
-      </c>
-      <c r="J24" t="s">
-        <v>66</v>
-      </c>
-      <c r="K24">
-        <v>5</v>
-      </c>
-      <c r="L24">
-        <v>48</v>
-      </c>
-      <c r="M24">
-        <v>6</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="9:15" x14ac:dyDescent="0.2">
-      <c r="I25">
-        <v>13</v>
-      </c>
-      <c r="J25" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25">
-        <v>5</v>
-      </c>
-      <c r="L25">
-        <v>58</v>
-      </c>
-      <c r="M25">
-        <v>6</v>
-      </c>
-      <c r="N25">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="18" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="10:15" x14ac:dyDescent="0.2">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
-    <sortCondition ref="C2:C7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L6:Q11">
+    <sortCondition ref="N6:N11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Plot for the second case
</commit_message>
<xml_diff>
--- a/Case 1/Case 1 - dummy data.xlsx
+++ b/Case 1/Case 1 - dummy data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B4678-CD1A-7F47-B064-CCD8D229DF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA14723-0607-D44D-903F-C93C3F4D6413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -1805,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2632,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
@@ -2697,13 +2697,13 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Schedule FIFO working perfectly
</commit_message>
<xml_diff>
--- a/Case 1/Case 1 - dummy data.xlsx
+++ b/Case 1/Case 1 - dummy data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7A8F51-146C-8145-BFDF-DF6AC72229D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114D5FE-8E86-C34D-BDD4-7877749C0D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="120">
   <si>
     <t>INFRASTRUCTURE</t>
   </si>
@@ -593,6 +593,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1805,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1867,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T8" t="s">
         <v>6</v>
@@ -2630,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2643,7 +2646,7 @@
     <col min="5" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -2665,179 +2668,140 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>54</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="C2">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>42</v>
-      </c>
-      <c r="E2">
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F5">
         <v>52</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1">
+        <v>48</v>
+      </c>
+      <c r="N5" s="1">
+        <v>6</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>43</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>53</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L6" s="1">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="1">
-        <v>5</v>
-      </c>
-      <c r="O6" s="1">
-        <v>42</v>
-      </c>
-      <c r="P6" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>3</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N7" s="1">
-        <v>5</v>
-      </c>
-      <c r="O7" s="1">
-        <v>48</v>
-      </c>
-      <c r="P7" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L8" s="1">
-        <v>13</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N8" s="1">
-        <v>5</v>
-      </c>
-      <c r="O8" s="1">
-        <v>54</v>
-      </c>
-      <c r="P8" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9">
-        <v>13</v>
-      </c>
-      <c r="M9" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9">
-        <v>6</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>6</v>
-      </c>
-      <c r="Q9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10">
-        <v>12</v>
-      </c>
-      <c r="M10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10">
-        <v>5</v>
-      </c>
-      <c r="O10">
-        <v>40</v>
-      </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11">
-        <v>6</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>6</v>
-      </c>
-      <c r="Q11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2862,8 +2826,8 @@
       <c r="O19" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L6:Q11">
-    <sortCondition ref="N6:N11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
+    <sortCondition ref="C2:C7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made small mistake in the create headway matrix closed, should also change this in S1
</commit_message>
<xml_diff>
--- a/Case 1/Case 1 - dummy data.xlsx
+++ b/Case 1/Case 1 - dummy data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114D5FE-8E86-C34D-BDD4-7877749C0D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C915EE4-87DC-6E41-88BA-EA3518A0303A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -593,9 +593,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2636,7 +2633,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2670,7 +2667,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
@@ -2679,19 +2676,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>66</v>
@@ -2700,96 +2697,96 @@
         <v>5</v>
       </c>
       <c r="D3" s="1">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
         <v>54</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <v>8</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>66</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>52</v>
-      </c>
-      <c r="J5" s="1">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="1">
-        <v>5</v>
-      </c>
-      <c r="M5" s="1">
-        <v>48</v>
-      </c>
-      <c r="N5" s="1">
-        <v>6</v>
-      </c>
-      <c r="O5" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>66</v>
       </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>

</xml_diff>